<commit_message>
update SerieA output files
</commit_message>
<xml_diff>
--- a/FantaSoccer/MyModule/SerieA/RealLineups_11.xlsx
+++ b/FantaSoccer/MyModule/SerieA/RealLineups_11.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="298">
   <si>
     <t>Atalanta</t>
   </si>
@@ -82,6 +82,9 @@
     <t>B. Djimsiti</t>
   </si>
   <si>
+    <t>G. Gasperini</t>
+  </si>
+  <si>
     <t>M. de Roon</t>
   </si>
   <si>
@@ -133,6 +136,9 @@
     <t>R. Soriano</t>
   </si>
   <si>
+    <t>S. Mihajlovic</t>
+  </si>
+  <si>
     <t>I. Mbaye</t>
   </si>
   <si>
@@ -154,6 +160,9 @@
     <t>N. Dominguez</t>
   </si>
   <si>
+    <t>F. Inzaghi</t>
+  </si>
+  <si>
     <t>P. Hetemaj</t>
   </si>
   <si>
@@ -199,6 +208,9 @@
     <t>R. Klavan</t>
   </si>
   <si>
+    <t>E. Di Francesco</t>
+  </si>
+  <si>
     <t>L. Pavoletti</t>
   </si>
   <si>
@@ -271,6 +283,9 @@
     <t>N. Milenkovic</t>
   </si>
   <si>
+    <t>P. Lirola</t>
+  </si>
+  <si>
     <t>M. Destro</t>
   </si>
   <si>
@@ -289,6 +304,9 @@
     <t>M. Perin</t>
   </si>
   <si>
+    <t>R. Maran</t>
+  </si>
+  <si>
     <t>E. Goldaniga</t>
   </si>
   <si>
@@ -346,6 +364,9 @@
     <t>S. Sensi</t>
   </si>
   <si>
+    <t>A. Conte</t>
+  </si>
+  <si>
     <t>N. Barella</t>
   </si>
   <si>
@@ -373,6 +394,9 @@
     <t>A. Rabiot</t>
   </si>
   <si>
+    <t>F. Bernardeschi</t>
+  </si>
+  <si>
     <t>M. de Ligt</t>
   </si>
   <si>
@@ -382,6 +406,9 @@
     <t>R. Bentancur</t>
   </si>
   <si>
+    <t>D. Kulusevski</t>
+  </si>
+  <si>
     <t>W. McKennie</t>
   </si>
   <si>
@@ -412,16 +439,19 @@
     <t>S. Milinkovic-Savic</t>
   </si>
   <si>
+    <t>M. Fares</t>
+  </si>
+  <si>
     <t>G. Escalante</t>
   </si>
   <si>
+    <t>Andreas Pereira</t>
+  </si>
+  <si>
     <t>J. Correa</t>
   </si>
   <si>
-    <t>M. Lazzari</t>
-  </si>
-  <si>
-    <t>A. Marusic</t>
+    <t>S. Inzaghi</t>
   </si>
   <si>
     <t>L. Marrone</t>
@@ -430,6 +460,9 @@
     <t>A. Cordaz</t>
   </si>
   <si>
+    <t>G. Stroppa</t>
+  </si>
+  <si>
     <t>S. Molina</t>
   </si>
   <si>
@@ -454,15 +487,15 @@
     <t>L. Magallan</t>
   </si>
   <si>
-    <t>M. Vulic</t>
-  </si>
-  <si>
     <t>Eduardo</t>
   </si>
   <si>
     <t>Pedro Pereira</t>
   </si>
   <si>
+    <t>S. Pioli</t>
+  </si>
+  <si>
     <t>A. Rebic</t>
   </si>
   <si>
@@ -502,6 +535,9 @@
     <t>J. Hauge</t>
   </si>
   <si>
+    <t>G. Gattuso</t>
+  </si>
+  <si>
     <t>F. Ghoulam</t>
   </si>
   <si>
@@ -562,6 +598,9 @@
     <t>S. Iacoponi</t>
   </si>
   <si>
+    <t>F. Liverani</t>
+  </si>
+  <si>
     <t>R. Gagliolo</t>
   </si>
   <si>
@@ -595,6 +634,9 @@
     <t>L. Spinazzola</t>
   </si>
   <si>
+    <t>Paulo Fonseca</t>
+  </si>
+  <si>
     <t>J. Veretout</t>
   </si>
   <si>
@@ -604,6 +646,9 @@
     <t>R. Karsdorp</t>
   </si>
   <si>
+    <t>Borja Mayoral</t>
+  </si>
+  <si>
     <t>M. Kumbulla</t>
   </si>
   <si>
@@ -628,6 +673,9 @@
     <t>A. Ekdal</t>
   </si>
   <si>
+    <t>C. Ranieri</t>
+  </si>
+  <si>
     <t>M. Yoshida</t>
   </si>
   <si>
@@ -661,6 +709,9 @@
     <t>D. Berardi</t>
   </si>
   <si>
+    <t>R. De Zerbi</t>
+  </si>
+  <si>
     <t>K. Ayhan</t>
   </si>
   <si>
@@ -700,6 +751,9 @@
     <t>C. Terzi</t>
   </si>
   <si>
+    <t>V. Italiano</t>
+  </si>
+  <si>
     <t>Diego Farias</t>
   </si>
   <si>
@@ -715,9 +769,6 @@
     <t>D. Verde</t>
   </si>
   <si>
-    <t>R. Marchizza</t>
-  </si>
-  <si>
     <t>G. Maggiore</t>
   </si>
   <si>
@@ -730,6 +781,9 @@
     <t>J. Chabot</t>
   </si>
   <si>
+    <t>K. Agudelo</t>
+  </si>
+  <si>
     <t>T. Rincon</t>
   </si>
   <si>
@@ -748,6 +802,9 @@
     <t>A. Belotti</t>
   </si>
   <si>
+    <t>M. Giampaolo</t>
+  </si>
+  <si>
     <t>A. Izzo</t>
   </si>
   <si>
@@ -784,6 +841,9 @@
     <t>B. Nuytinck</t>
   </si>
   <si>
+    <t>L. Gotti</t>
+  </si>
+  <si>
     <t>K. Bonifazi</t>
   </si>
   <si>
@@ -832,6 +892,9 @@
     <t>A. Favilli</t>
   </si>
   <si>
+    <t>I. Juric</t>
+  </si>
+  <si>
     <t>A. Barak</t>
   </si>
   <si>
@@ -842,6 +905,9 @@
   </si>
   <si>
     <t>M. Lovato</t>
+  </si>
+  <si>
+    <t>E. Colley</t>
   </si>
 </sst>
 </file>
@@ -1199,7 +1265,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U14"/>
+  <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1275,61 +1341,61 @@
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="G2" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="H2" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="I2" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="J2" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="K2" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="L2" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="M2" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="N2" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="O2" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
       <c r="P2" t="s">
-        <v>199</v>
+        <v>214</v>
       </c>
       <c r="Q2" t="s">
-        <v>212</v>
+        <v>228</v>
       </c>
       <c r="R2" t="s">
-        <v>225</v>
+        <v>242</v>
       </c>
       <c r="S2" t="s">
-        <v>238</v>
+        <v>256</v>
       </c>
       <c r="T2" t="s">
-        <v>251</v>
+        <v>270</v>
       </c>
       <c r="U2" t="s">
-        <v>264</v>
+        <v>284</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -1340,61 +1406,61 @@
         <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F3" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="G3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="H3" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="I3" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="J3" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="K3" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="L3" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="M3" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="N3" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="O3" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="P3" t="s">
-        <v>200</v>
+        <v>215</v>
       </c>
       <c r="Q3" t="s">
-        <v>213</v>
+        <v>229</v>
       </c>
       <c r="R3" t="s">
-        <v>226</v>
+        <v>243</v>
       </c>
       <c r="S3" t="s">
-        <v>239</v>
+        <v>257</v>
       </c>
       <c r="T3" t="s">
-        <v>252</v>
+        <v>271</v>
       </c>
       <c r="U3" t="s">
-        <v>265</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -1405,61 +1471,61 @@
         <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F4" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="G4" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="H4" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="I4" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="J4" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="K4" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="L4" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="M4" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="N4" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="O4" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
       <c r="P4" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="Q4" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="R4" t="s">
-        <v>227</v>
+        <v>244</v>
       </c>
       <c r="S4" t="s">
-        <v>240</v>
+        <v>258</v>
       </c>
       <c r="T4" t="s">
-        <v>253</v>
+        <v>272</v>
       </c>
       <c r="U4" t="s">
-        <v>266</v>
+        <v>286</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -1470,61 +1536,61 @@
         <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F5" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="G5" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="H5" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="I5" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="J5" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="K5" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="L5" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="M5" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="N5" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="O5" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="P5" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="Q5" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
       <c r="R5" t="s">
-        <v>228</v>
+        <v>245</v>
       </c>
       <c r="S5" t="s">
-        <v>241</v>
+        <v>259</v>
       </c>
       <c r="T5" t="s">
-        <v>254</v>
+        <v>273</v>
       </c>
       <c r="U5" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -1535,61 +1601,61 @@
         <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="G6" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="H6" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="I6" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="J6" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="K6" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="L6" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="M6" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="N6" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="O6" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="P6" t="s">
-        <v>203</v>
+        <v>218</v>
       </c>
       <c r="Q6" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
       <c r="R6" t="s">
-        <v>229</v>
+        <v>246</v>
       </c>
       <c r="S6" t="s">
-        <v>242</v>
+        <v>260</v>
       </c>
       <c r="T6" t="s">
-        <v>255</v>
+        <v>274</v>
       </c>
       <c r="U6" t="s">
-        <v>268</v>
+        <v>288</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -1600,61 +1666,61 @@
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F7" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="G7" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="H7" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="I7" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="J7" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="K7" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="L7" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="M7" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="N7" t="s">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="O7" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
       <c r="P7" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
       <c r="Q7" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
       <c r="R7" t="s">
-        <v>230</v>
+        <v>247</v>
       </c>
       <c r="S7" t="s">
-        <v>243</v>
+        <v>261</v>
       </c>
       <c r="T7" t="s">
-        <v>256</v>
+        <v>275</v>
       </c>
       <c r="U7" t="s">
-        <v>269</v>
+        <v>289</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -1665,61 +1731,61 @@
         <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E8" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F8" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="G8" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="H8" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="I8" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="J8" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="K8" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="L8" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="M8" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="N8" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="O8" t="s">
-        <v>194</v>
+        <v>207</v>
       </c>
       <c r="P8" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="Q8" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
       <c r="R8" t="s">
-        <v>231</v>
+        <v>248</v>
       </c>
       <c r="S8" t="s">
-        <v>244</v>
+        <v>262</v>
       </c>
       <c r="T8" t="s">
-        <v>257</v>
+        <v>276</v>
       </c>
       <c r="U8" t="s">
-        <v>270</v>
+        <v>290</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -1730,61 +1796,61 @@
         <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E9" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F9" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="G9" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="H9" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="I9" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="J9" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="K9" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="L9" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="M9" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="N9" t="s">
-        <v>182</v>
+        <v>194</v>
       </c>
       <c r="O9" t="s">
-        <v>94</v>
+        <v>208</v>
       </c>
       <c r="P9" t="s">
-        <v>206</v>
+        <v>221</v>
       </c>
       <c r="Q9" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
       <c r="R9" t="s">
-        <v>232</v>
+        <v>249</v>
       </c>
       <c r="S9" t="s">
-        <v>245</v>
+        <v>263</v>
       </c>
       <c r="T9" t="s">
-        <v>258</v>
+        <v>277</v>
       </c>
       <c r="U9" t="s">
-        <v>271</v>
+        <v>291</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -1795,61 +1861,61 @@
         <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E10" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F10" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="G10" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="H10" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="I10" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="J10" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="K10" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="L10" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="M10" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="N10" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="O10" t="s">
-        <v>195</v>
+        <v>100</v>
       </c>
       <c r="P10" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="Q10" t="s">
-        <v>220</v>
+        <v>236</v>
       </c>
       <c r="R10" t="s">
-        <v>233</v>
+        <v>250</v>
       </c>
       <c r="S10" t="s">
-        <v>246</v>
+        <v>264</v>
       </c>
       <c r="T10" t="s">
-        <v>259</v>
+        <v>278</v>
       </c>
       <c r="U10" t="s">
-        <v>272</v>
+        <v>292</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -1860,61 +1926,61 @@
         <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E11" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F11" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G11" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="H11" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="I11" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="J11" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="K11" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="L11" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="M11" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="N11" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="O11" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
       <c r="P11" t="s">
-        <v>208</v>
+        <v>223</v>
       </c>
       <c r="Q11" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
       <c r="R11" t="s">
-        <v>234</v>
+        <v>251</v>
       </c>
       <c r="S11" t="s">
-        <v>247</v>
+        <v>265</v>
       </c>
       <c r="T11" t="s">
-        <v>260</v>
+        <v>279</v>
       </c>
       <c r="U11" t="s">
-        <v>273</v>
+        <v>293</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -1925,61 +1991,61 @@
         <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F12" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="G12" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="H12" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="I12" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="J12" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="K12" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="L12" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="M12" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="N12" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="O12" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="P12" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="Q12" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
       <c r="R12" t="s">
-        <v>235</v>
+        <v>252</v>
       </c>
       <c r="S12" t="s">
-        <v>248</v>
+        <v>266</v>
       </c>
       <c r="T12" t="s">
-        <v>261</v>
+        <v>280</v>
       </c>
       <c r="U12" t="s">
-        <v>274</v>
+        <v>294</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -1990,61 +2056,61 @@
         <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E13" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F13" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="G13" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="H13" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="I13" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="J13" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="K13" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="L13" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="M13" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="N13" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="O13" t="s">
-        <v>198</v>
+        <v>211</v>
       </c>
       <c r="P13" t="s">
-        <v>210</v>
+        <v>225</v>
       </c>
       <c r="Q13" t="s">
-        <v>223</v>
+        <v>239</v>
       </c>
       <c r="R13" t="s">
-        <v>236</v>
+        <v>253</v>
       </c>
       <c r="S13" t="s">
-        <v>249</v>
+        <v>267</v>
       </c>
       <c r="T13" t="s">
-        <v>262</v>
+        <v>281</v>
       </c>
       <c r="U13" t="s">
-        <v>275</v>
+        <v>295</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -2055,52 +2121,123 @@
         <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E14" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F14" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="G14" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="H14" t="s">
-        <v>110</v>
+        <v>116</v>
+      </c>
+      <c r="I14" t="s">
+        <v>130</v>
       </c>
       <c r="J14" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="K14" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="L14" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="M14" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="N14" t="s">
-        <v>187</v>
+        <v>199</v>
+      </c>
+      <c r="O14" t="s">
+        <v>212</v>
       </c>
       <c r="P14" t="s">
-        <v>211</v>
+        <v>226</v>
       </c>
       <c r="Q14" t="s">
-        <v>224</v>
+        <v>240</v>
       </c>
       <c r="R14" t="s">
-        <v>237</v>
+        <v>254</v>
       </c>
       <c r="S14" t="s">
-        <v>250</v>
+        <v>268</v>
       </c>
       <c r="T14" t="s">
-        <v>263</v>
+        <v>282</v>
+      </c>
+      <c r="U14" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" t="s">
+        <v>89</v>
+      </c>
+      <c r="G15" t="s">
+        <v>103</v>
+      </c>
+      <c r="H15" t="s">
+        <v>117</v>
+      </c>
+      <c r="I15" t="s">
+        <v>131</v>
+      </c>
+      <c r="J15" t="s">
+        <v>145</v>
+      </c>
+      <c r="L15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M15" t="s">
+        <v>186</v>
+      </c>
+      <c r="N15" t="s">
+        <v>200</v>
+      </c>
+      <c r="O15" t="s">
+        <v>213</v>
+      </c>
+      <c r="P15" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>241</v>
+      </c>
+      <c r="R15" t="s">
+        <v>255</v>
+      </c>
+      <c r="S15" t="s">
+        <v>269</v>
+      </c>
+      <c r="T15" t="s">
+        <v>283</v>
+      </c>
+      <c r="U15" t="s">
+        <v>297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>